<commit_message>
Actualizacion de nombre y cerrar sesion y agregar campo de MMOO
</commit_message>
<xml_diff>
--- a/static/importar_cotizaciones.xlsx
+++ b/static/importar_cotizaciones.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisg\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisg\OneDrive\Escritorio\APP\gz_services\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDC1E6D-3E4B-472E-A2AF-D310D66A9711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BB760A-BAAD-4AA9-A25F-08674F6E4D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2204AF21-E8DF-4128-86E2-25C7980E1F52}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID CLARO</t>
   </si>
@@ -52,13 +52,16 @@
   </si>
   <si>
     <t>MONTO COTIZADO</t>
+  </si>
+  <si>
+    <t>MONTO MMOO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +74,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,17 +106,17 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0B2430-6898-4998-A70C-D1521C2B2CC7}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,26 +447,30 @@
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -463,108 +478,55 @@
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>